<commit_message>
fix: atualiza planilha de gastos do t3
</commit_message>
<xml_diff>
--- a/T3/Planilha de gastos T3 Microcontroladores.xlsx
+++ b/T3/Planilha de gastos T3 Microcontroladores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7383BF-5E80-4972-AC30-9AA6C0C45FDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A7ED0C-6C7F-41DC-BDA7-251B22876AFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{0A4BA978-FADF-4657-93F8-56D64A58906B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Tabela de preços</t>
   </si>
@@ -34,21 +34,6 @@
   </si>
   <si>
     <t>Custo</t>
-  </si>
-  <si>
-    <t>Display touch Raspberry Pi 720 x 1280</t>
-  </si>
-  <si>
-    <t>Raspberry Pi 4GB Ram</t>
-  </si>
-  <si>
-    <t>Jumpers Macho Macho (40 unidades)</t>
-  </si>
-  <si>
-    <t>Protoboard 170 pontos</t>
-  </si>
-  <si>
-    <t>Cartão SD 128 GB</t>
   </si>
   <si>
     <t>Custo Total</t>
@@ -62,7 +47,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -137,18 +122,18 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -464,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DFBEA4-7365-4505-8989-72CFA4D8EB73}">
-  <dimension ref="D6:E14"/>
+  <dimension ref="D6:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,73 +462,34 @@
   </cols>
   <sheetData>
     <row r="6" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="6">
-        <v>759.05</v>
+      <c r="D8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="5">
+        <v>45.53</v>
       </c>
     </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="6">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="10" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="6">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="11" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="6">
-        <v>4.59</v>
-      </c>
-    </row>
-    <row r="12" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="6">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="6">
+      <c r="D9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2">
+        <f>SUM(E8)</f>
         <v>45.53</v>
-      </c>
-    </row>
-    <row r="14" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1439.32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>